<commit_message>
added the dropped cells from the cap cutouts
</commit_message>
<xml_diff>
--- a/masks/code/TKIDModule_spreadsheet_20200512_AW.xlsx
+++ b/masks/code/TKIDModule_spreadsheet_20200512_AW.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13665" windowHeight="7425" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13665" windowHeight="7425"/>
   </bookViews>
   <sheets>
     <sheet name="Patches" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="287">
   <si>
     <t>AGA Marks</t>
   </si>
@@ -880,6 +880,9 @@
   <si>
     <t>Drop R1C1, R1C3, R1C5, R2C2, R2C4</t>
   </si>
+  <si>
+    <t>Drop R1C1, R1C2, R1C9, R2C1, R2C8, R2C9. R3C9, R4C1, R7C9, R8C1, R11C9, R12C1, R15C1, R15C9, R16C1, R16C9</t>
+  </si>
 </sst>
 </file>
 
@@ -939,8 +942,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1255,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:AC155"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="AC67" sqref="AC67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1594,18 +1600,18 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="3" t="s">
+      <c r="T12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="3" t="s">
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AA12" s="4"/>
+      <c r="AA12" s="5"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
     </row>
@@ -1613,50 +1619,50 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="3" t="s">
+      <c r="G13" s="5"/>
+      <c r="H13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="3" t="s">
+      <c r="M13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="3" t="s">
+      <c r="N13" s="5"/>
+      <c r="O13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P13" s="4"/>
+      <c r="P13" s="5"/>
       <c r="Q13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="3" t="s">
+      <c r="T13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="U13" s="4"/>
-      <c r="V13" s="3" t="s">
+      <c r="U13" s="5"/>
+      <c r="V13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="W13" s="4"/>
-      <c r="X13" s="3" t="s">
+      <c r="W13" s="5"/>
+      <c r="X13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="3" t="s">
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AA13" s="4"/>
+      <c r="AA13" s="5"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
     </row>
@@ -4014,7 +4020,9 @@
       <c r="AB45" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AC45" s="1"/>
+      <c r="AC45" s="1" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
@@ -5563,7 +5571,9 @@
       <c r="AB66" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AC66" s="1"/>
+      <c r="AC66" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="67" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
@@ -5638,7 +5648,9 @@
       <c r="AB67" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AC67" s="1"/>
+      <c r="AC67" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="68" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
@@ -12064,17 +12076,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="O13:P13"/>
     <mergeCell ref="T12:Y12"/>
     <mergeCell ref="T13:U13"/>
     <mergeCell ref="V13:W13"/>
     <mergeCell ref="X13:Y13"/>
     <mergeCell ref="Z12:AA12"/>
     <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="O13:P13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -12111,18 +12123,18 @@
     <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="H1" s="4"/>
+      <c r="H1" s="5"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
         <v>270</v>
@@ -27748,7 +27760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -27779,68 +27791,68 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="3" t="s">
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="4"/>
+      <c r="AA1" s="5"/>
       <c r="AB1" s="1"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="3" t="s">
+      <c r="N2" s="5"/>
+      <c r="O2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="4"/>
+      <c r="P2" s="5"/>
       <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="3" t="s">
+      <c r="U2" s="5"/>
+      <c r="V2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="4"/>
-      <c r="X2" s="3" t="s">
+      <c r="W2" s="5"/>
+      <c r="X2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="3" t="s">
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AA2" s="4"/>
+      <c r="AA2" s="5"/>
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.45">

</xml_diff>